<commit_message>
get ready for branch
</commit_message>
<xml_diff>
--- a/TestableConsoleApp/Backlog.xlsx
+++ b/TestableConsoleApp/Backlog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>Logging</t>
+  </si>
+  <si>
+    <t>Get order history from console</t>
+  </si>
+  <si>
+    <t>Add users</t>
+  </si>
+  <si>
+    <t>Add resource to foods and drinks</t>
+  </si>
+  <si>
+    <t>Add current culture to price to console</t>
+  </si>
+  <si>
+    <t>Committed</t>
+  </si>
+  <si>
+    <t>Let user change language</t>
   </si>
 </sst>
 </file>
@@ -430,15 +448,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="82.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -476,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -498,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -542,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -590,6 +608,61 @@
       </c>
       <c r="C13" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>